<commit_message>
Css and counterfactual explanation added
</commit_message>
<xml_diff>
--- a/my_variable.xlsx
+++ b/my_variable.xlsx
@@ -61,7 +61,7 @@
     <t>Tax Liens</t>
   </si>
   <si>
-    <t>10000</t>
+    <t>140174</t>
   </si>
   <si>
     <t>1</t>
@@ -70,22 +70,22 @@
     <t>200</t>
   </si>
   <si>
-    <t>500000000</t>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8000</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>53</t>
+  </si>
+  <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>50000000</t>
   </si>
 </sst>
 </file>
@@ -510,22 +510,22 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
@@ -534,13 +534,13 @@
         <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final product in balanced dataset
</commit_message>
<xml_diff>
--- a/my_variable.xlsx
+++ b/my_variable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Current Loan Amount</t>
   </si>
@@ -61,7 +61,7 @@
     <t>Tax Liens</t>
   </si>
   <si>
-    <t>140174</t>
+    <t>10000</t>
   </si>
   <si>
     <t>1</t>
@@ -73,19 +73,22 @@
     <t>1600</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>8000</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
     <t>53</t>
   </si>
   <si>
-    <t>0</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -510,37 +513,37 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>